<commit_message>
_m12TAk3r , 8:17AM , 14112018
</commit_message>
<xml_diff>
--- a/DatabaseExcel/GiangVien.xlsx
+++ b/DatabaseExcel/GiangVien.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\QuanLyDiem\DatabaseExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GITT\QuanLyDiem\DatabaseExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65184499-A9EA-4C39-8F9A-207F3784CC07}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>GV001</t>
   </si>
@@ -124,12 +123,60 @@
   </si>
   <si>
     <t>0964000582</t>
+  </si>
+  <si>
+    <t>12011979</t>
+  </si>
+  <si>
+    <t>13011980</t>
+  </si>
+  <si>
+    <t>27051979</t>
+  </si>
+  <si>
+    <t>30031985</t>
+  </si>
+  <si>
+    <t>19011979</t>
+  </si>
+  <si>
+    <t>31101979</t>
+  </si>
+  <si>
+    <t>14121981</t>
+  </si>
+  <si>
+    <t>16101975</t>
+  </si>
+  <si>
+    <t>21 Nguyễn Lương Bằng</t>
+  </si>
+  <si>
+    <t>30 Lương Nhữ Hộc</t>
+  </si>
+  <si>
+    <t>1 Nguyễn Tri Phương</t>
+  </si>
+  <si>
+    <t>80 Trưng Nữ Vương</t>
+  </si>
+  <si>
+    <t>25 Bạch Đằng</t>
+  </si>
+  <si>
+    <t>60  Lê Lợi</t>
+  </si>
+  <si>
+    <t>40 Đào Cam Mộc</t>
+  </si>
+  <si>
+    <t>12 Núi Thành</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,10 +215,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -452,166 +500,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="3">
+        <v>28867</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3">
+        <v>29233</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="3">
+        <v>29934</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3">
+        <v>29159</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3">
+        <v>27683</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3">
+        <v>29002</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3">
+        <v>31136</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3">
+        <v>28874</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId9"/>

</xml_diff>